<commit_message>
WIP - Complex Policy Test Scenario
</commit_message>
<xml_diff>
--- a/VaultAgent/Documentation/VaultPolicyTestResults.xlsx
+++ b/VaultAgent/Documentation/VaultPolicyTestResults.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\A_Dev\OpenSource\vaultapi\VaultAgent\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\A_Dev\VaultAPI\VaultAgent\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="35">
   <si>
     <t>beA/path1</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>Saving subSecrets always use /*</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>beA/path1/ {Attrib}</t>
+  </si>
+  <si>
+    <t>CRUD</t>
   </si>
 </sst>
 </file>
@@ -471,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,10 +519,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -527,10 +536,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -544,7 +553,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -562,7 +571,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -572,20 +581,21 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
-        <v>13</v>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>